<commit_message>
Report formulas & format
</commit_message>
<xml_diff>
--- a/templates/report/dashboard.xlsx
+++ b/templates/report/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78DA9E8-50E4-4F6A-A1FF-A7C656015ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10C5866-13A8-40AD-957F-C46DE12C0D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Reservas</t>
   </si>
@@ -47,6 +47,9 @@
   <si>
     <t>Fecha
 check-in</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -115,23 +118,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -151,25 +143,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -560,49 +556,55 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35" style="2" customWidth="1"/>
-    <col min="3" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="35" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="24.85546875" style="2"/>
+    <col min="1" max="1" width="24.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="1" customWidth="1"/>
+    <col min="3" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="35" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="24.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>